<commit_message>
minor notation fixed in beta binomial
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71717A79-E5A7-B345-B9AA-C3305710918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB84307-794A-F148-AE7B-41150A01AA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Previsione</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>ripresa bayes rule (marginal, joint; fatto risolvere esempio infected | positive;  goat)</t>
+  </si>
+  <si>
+    <t>exe 3.9 3.10??</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,6 +849,9 @@
         <f>E6+7</f>
         <v>45194</v>
       </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">

</xml_diff>

<commit_message>
updated solutions in the normal normal, added formalization of the hyppocampus model
updated solutions in the normal normal, added formalization of the hyppocampus model
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB84307-794A-F148-AE7B-41150A01AA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D3C2D2-2DBB-784A-A8EE-66437668B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Previsione</t>
   </si>
@@ -154,13 +154,19 @@
     <t>MF exe MCMC; finito in lieve anticipo</t>
   </si>
   <si>
-    <t>anticipare qui presentazione progetto??</t>
-  </si>
-  <si>
     <t>ripresa bayes rule (marginal, joint; fatto risolvere esempio infected | positive;  goat)</t>
   </si>
   <si>
-    <t>exe 3.9 3.10??</t>
+    <t>beta-binomial (beta; con esercizio di tune prior  e inizio 3.9)</t>
+  </si>
+  <si>
+    <t>presentare assignment e progetto</t>
+  </si>
+  <si>
+    <t>ripresa beta; binomial likelihood; up to slide 58 (sensitivity to the prior)</t>
+  </si>
+  <si>
+    <t>gc: guardare come inserire test ipotesi di francesca</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +261,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -287,7 +299,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -327,6 +339,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -738,7 +753,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,7 +842,7 @@
         <v>45190</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -849,8 +864,8 @@
         <f>E6+7</f>
         <v>45194</v>
       </c>
-      <c r="F8" t="s">
-        <v>40</v>
+      <c r="F8" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -869,6 +884,9 @@
         <v>7</v>
       </c>
       <c r="E9" s="4"/>
+      <c r="F9" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -885,8 +903,8 @@
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>38</v>
+      <c r="F10" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -905,6 +923,9 @@
         <v>9</v>
       </c>
       <c r="E11" s="4"/>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -922,6 +943,9 @@
         <v>10</v>
       </c>
       <c r="E12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -956,6 +980,9 @@
         <v>11</v>
       </c>
       <c r="E14" s="4"/>
+      <c r="F14" s="16" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -990,6 +1017,9 @@
         <v>12</v>
       </c>
       <c r="E16" s="4"/>
+      <c r="F16" s="19" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">

</xml_diff>

<commit_message>
clean up of prob programming
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D766B0-F500-9549-8BB3-405336D79693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9F71D-BF35-EE4A-91B4-DB97AC279521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Previsione</t>
   </si>
@@ -175,7 +175,19 @@
     <t>exe MF</t>
   </si>
   <si>
-    <t>presentare  progetto</t>
+    <t xml:space="preserve"> MCMC facendo poi implementare island hopping</t>
+  </si>
+  <si>
+    <t>chiudere MCMC, prob programming</t>
+  </si>
+  <si>
+    <t>prob programming, presentare  progetto</t>
+  </si>
+  <si>
+    <t>normal-normal</t>
+  </si>
+  <si>
+    <t>hyp test</t>
   </si>
 </sst>
 </file>
@@ -761,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1027,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1035,7 +1047,7 @@
         <v>45218</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1057,8 +1069,8 @@
         <f>E14+7</f>
         <v>45222</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>45</v>
+      <c r="F16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1080,6 +1092,9 @@
         <f>E15+7</f>
         <v>45225</v>
       </c>
+      <c r="F17" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1096,7 +1111,13 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="14">
+        <f>E16+7</f>
+        <v>45229</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1113,7 +1134,13 @@
       <c r="D19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="14">
+        <f>E17+7</f>
+        <v>45232</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1130,7 +1157,13 @@
       <c r="D20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="14">
+        <f>E18+7</f>
+        <v>45236</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">

</xml_diff>

<commit_message>
minor adjustment su rope
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9F71D-BF35-EE4A-91B4-DB97AC279521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BEC0F0-813A-A94D-90B2-5A2869119446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Previsione</t>
   </si>
@@ -178,16 +178,19 @@
     <t xml:space="preserve"> MCMC facendo poi implementare island hopping</t>
   </si>
   <si>
-    <t>chiudere MCMC, prob programming</t>
-  </si>
-  <si>
-    <t>prob programming, presentare  progetto</t>
-  </si>
-  <si>
-    <t>normal-normal</t>
-  </si>
-  <si>
     <t>hyp test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>chiuso MCMC, prob programming (fino a cambiare prior beta(1,1) con uniform)</t>
+  </si>
+  <si>
+    <t>normal-normal (ultimi 15 min presentare progetto)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prob programming (finire nbook 1 con rope);  ultimi 15 min presenta assignment </t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="14">
-        <f>E13+7</f>
+        <f t="shared" ref="E15:E20" si="2">E13+7</f>
         <v>45218</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -1066,11 +1069,11 @@
         <v>12</v>
       </c>
       <c r="E16" s="14">
-        <f>E14+7</f>
+        <f t="shared" si="2"/>
         <v>45222</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1089,7 +1092,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="14">
-        <f>E15+7</f>
+        <f t="shared" si="2"/>
         <v>45225</v>
       </c>
       <c r="F17" s="11" t="s">
@@ -1112,11 +1115,11 @@
         <v>15</v>
       </c>
       <c r="E18" s="14">
-        <f>E16+7</f>
+        <f t="shared" si="2"/>
         <v>45229</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1135,11 +1138,11 @@
         <v>37</v>
       </c>
       <c r="E19" s="14">
-        <f>E17+7</f>
+        <f t="shared" si="2"/>
         <v>45232</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1158,11 +1161,11 @@
         <v>16</v>
       </c>
       <c r="E20" s="14">
-        <f>E18+7</f>
+        <f t="shared" si="2"/>
         <v>45236</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1181,6 +1184,9 @@
         <v>14</v>
       </c>
       <c r="E21" s="4"/>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">

</xml_diff>

<commit_message>
fixed explanation of making decisions with rope
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BEC0F0-813A-A94D-90B2-5A2869119446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAD0D68-5B2B-8C47-8717-DE40CE8FB8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
     <t>normal-normal (ultimi 15 min presentare progetto)</t>
   </si>
   <si>
-    <t xml:space="preserve">prob programming (finire nbook 1 con rope);  ultimi 15 min presenta assignment </t>
+    <t xml:space="preserve">finito nbook 1 con rope;  ultimi 15 min presenta assignment </t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -363,9 +363,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -777,7 +778,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,7 +1142,7 @@
         <f t="shared" si="2"/>
         <v>45232</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="20" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update test, reworking the example on the beta-blocker to insert the rope
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C10F80E-554D-B145-949B-826CF6D65980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6D4C0A-324E-0144-8D5F-88F3831EAC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Previsione</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>hyp test tradizionali (1 sample, 2 samples); test bayesiani</t>
+  </si>
+  <si>
+    <t>recap test 2 campioni; it- test bayesiano</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -262,6 +265,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -317,7 +326,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -357,6 +366,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1037,7 +1049,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" ref="E15:E23" si="2">E13+7</f>
+        <f t="shared" ref="E15:E24" si="2">E13+7</f>
         <v>45218</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -1224,8 +1236,8 @@
         <f t="shared" si="2"/>
         <v>45246</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>18</v>
+      <c r="F23" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1243,7 +1255,13 @@
       <c r="D24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="14">
+        <f t="shared" si="2"/>
+        <v>45250</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">

</xml_diff>

<commit_message>
update to bayesiaan t-test (introdotto anche soluzione frequentista)
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6D4C0A-324E-0144-8D5F-88F3831EAC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E647FC-7D46-5F45-B874-B5BF33E96E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Previsione</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>recap test 2 campioni; it- test bayesiano</t>
+  </si>
+  <si>
+    <t>revisione progetti + dire Master DS</t>
+  </si>
+  <si>
+    <t>test bayesiani</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,7 +1055,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" ref="E15:E24" si="2">E13+7</f>
+        <f t="shared" ref="E15:E33" si="2">E13+7</f>
         <v>45218</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -1260,7 +1266,7 @@
         <v>45250</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1278,7 +1284,10 @@
       <c r="D25" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="14">
+        <f t="shared" si="2"/>
+        <v>45253</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -1295,9 +1304,12 @@
       <c r="D26" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="14">
+        <f t="shared" si="2"/>
+        <v>45257</v>
+      </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1315,7 +1327,10 @@
       <c r="D27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="14">
+        <f t="shared" si="2"/>
+        <v>45260</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1332,7 +1347,10 @@
       <c r="D28" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="14">
+        <f t="shared" si="2"/>
+        <v>45264</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1349,7 +1367,10 @@
       <c r="D29" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="14">
+        <f t="shared" si="2"/>
+        <v>45267</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1366,7 +1387,13 @@
       <c r="D30" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="14">
+        <f t="shared" si="2"/>
+        <v>45271</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1383,7 +1410,10 @@
       <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="14">
+        <f t="shared" si="2"/>
+        <v>45274</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -1400,9 +1430,12 @@
       <c r="D32" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="14">
+        <f t="shared" si="2"/>
+        <v>45278</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1413,6 +1446,13 @@
       </c>
       <c r="D33" t="s">
         <v>23</v>
+      </c>
+      <c r="E33" s="14">
+        <f t="shared" si="2"/>
+        <v>45281</v>
+      </c>
+      <c r="F33" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight chnage to hierarchical model
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E647FC-7D46-5F45-B874-B5BF33E96E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A718F8-FC99-F44C-B616-C4E5CAC1BD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
     <t>revisione progetti + dire Master DS</t>
   </si>
   <si>
-    <t>test bayesiani</t>
+    <t>test bayesiani (modello robusto e posterior predictive checks)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
minor fix al modello gerarchico
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A272891-AACF-3148-B13F-50F97FB7A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFCE180-041F-734D-9E6A-6C1C6753E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Previsione</t>
   </si>
@@ -163,9 +163,6 @@
     <t>ripresa beta; binomial likelihood; up to slide 58 (sensitivity to the prior)</t>
   </si>
   <si>
-    <t>modelli gerarchici: dire possibilità di fare tesi su ANN gerarchica</t>
-  </si>
-  <si>
     <t xml:space="preserve"> normal normal</t>
   </si>
   <si>
@@ -196,16 +193,19 @@
     <t>recap test 2 campioni; it- test bayesiano</t>
   </si>
   <si>
-    <t>revisione progetti + dire Master DS</t>
-  </si>
-  <si>
     <t>test bayesiani (modello robusto e posterior predictive checks)</t>
   </si>
   <si>
     <t>pooled e unpooled model</t>
   </si>
   <si>
-    <t>hierarchical spotify (partendo dal typing example)</t>
+    <t>revisione progetti + dire Master DS e possibilità tesi su ANN gerarchiche</t>
+  </si>
+  <si>
+    <t>hierarchical  (predizione per known and unknown artist, shrinkage, typing exam)</t>
+  </si>
+  <si>
+    <t>riprendi hierarchical, regression</t>
   </si>
 </sst>
 </file>
@@ -996,7 +996,7 @@
         <v>45208</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
         <v>45211</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>45215</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1065,7 +1065,7 @@
         <v>45218</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1088,7 +1088,7 @@
         <v>45222</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1111,7 +1111,7 @@
         <v>45225</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,7 +1134,7 @@
         <v>45229</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1157,7 +1157,7 @@
         <v>45232</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
         <v>45236</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1203,7 +1203,7 @@
         <v>45239</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1226,7 +1226,7 @@
         <v>45243</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>45246</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1272,7 +1272,7 @@
         <v>45250</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1315,7 +1315,7 @@
         <v>45257</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
         <v>45260</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1360,6 +1360,9 @@
         <f t="shared" si="2"/>
         <v>45264</v>
       </c>
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1380,6 +1383,9 @@
         <f t="shared" si="2"/>
         <v>45267</v>
       </c>
+      <c r="F29" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1400,9 +1406,6 @@
         <f t="shared" si="2"/>
         <v>45271</v>
       </c>
-      <c r="F30" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1461,7 +1464,7 @@
         <v>45281</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fix in lienar regression, added my python code for assignemnt solution
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046DBD4E-B648-8744-BB5F-03EA1E1A79F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EEA5DA-9C70-EB4D-BF6F-EEA83A2444EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Previsione</t>
   </si>
@@ -199,16 +199,16 @@
     <t>pooled e unpooled model</t>
   </si>
   <si>
-    <t>revisione progetti + dire Master DS e possibilità tesi su ANN gerarchiche</t>
-  </si>
-  <si>
     <t>hierarchical  (predizione per known and unknown artist, shrinkage, typing exam)</t>
   </si>
   <si>
     <t>linear regression (esempio bike rides, fit pymc3, model visualization)</t>
   </si>
   <si>
-    <t>riprendere lin reg</t>
+    <t>valutazione didattica, revisione progetti, presenta Master DS e possibilità tesi su ANN bayesiane e  gerarchiche</t>
+  </si>
+  <si>
+    <t>lin reg</t>
   </si>
 </sst>
 </file>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1341,7 @@
         <v>45260</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
         <v>45264</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1432,6 +1432,9 @@
         <f t="shared" si="2"/>
         <v>45274</v>
       </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -1452,6 +1455,9 @@
         <f t="shared" si="2"/>
         <v>45278</v>
       </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33">
@@ -1470,7 +1476,7 @@
         <v>45281</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed beta -> beta_county in varying slope model
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenza lezioni BDA.xlsx
+++ b/syllabus-and-improv/sequenza lezioni BDA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EEA5DA-9C70-EB4D-BF6F-EEA83A2444EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AADE68-7172-A945-96F1-033B42678ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Previsione</t>
   </si>
@@ -205,10 +205,13 @@
     <t>linear regression (esempio bike rides, fit pymc3, model visualization)</t>
   </si>
   <si>
-    <t>valutazione didattica, revisione progetti, presenta Master DS e possibilità tesi su ANN bayesiane e  gerarchiche</t>
-  </si>
-  <si>
     <t>lin reg</t>
+  </si>
+  <si>
+    <t>reg gerarchica</t>
+  </si>
+  <si>
+    <t>reg gerarchica, valutazione didattica, Master DS, possiblità tesi du ANN bayesiane e gerarchiche</t>
   </si>
 </sst>
 </file>
@@ -795,7 +798,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D16" zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1413,7 @@
         <v>45271</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1433,7 +1436,7 @@
         <v>45274</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1456,7 +1459,7 @@
         <v>45278</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
@@ -1476,7 +1479,7 @@
         <v>45281</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>